<commit_message>
Draft FADA database changes for discussion
The draft FADA database changes document is still a work in progress,
but I committed the changes for discussion.
</commit_message>
<xml_diff>
--- a/database-info/Field_mapping.xlsx
+++ b/database-info/Field_mapping.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaikedewever/Documents/fada-import-specs/database-info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="14440" yWindow="3840" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,18 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="0" iterate="1" concurrentCalc="0"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="268">
   <si>
     <t>id</t>
   </si>
@@ -123,7 +133,7 @@
     <t>Faunistic</t>
   </si>
   <si>
-    <t>New field in fada.species or in new speciesprofile table? </t>
+    <t>New field in fada.species or in new speciesprofile table?</t>
   </si>
   <si>
     <t>Distribution</t>
@@ -160,36 +170,703 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>xls-order</t>
+  </si>
+  <si>
+    <t>xls-sheet</t>
+  </si>
+  <si>
+    <t>xls-field</t>
+  </si>
+  <si>
+    <t>DwC-Core_or_Extension</t>
+  </si>
+  <si>
+    <t>DwC-Term_name</t>
+  </si>
+  <si>
+    <t>fada.taxons</t>
+  </si>
+  <si>
+    <t>fada.taxons-Comments</t>
+  </si>
+  <si>
+    <t>fada.species</t>
+  </si>
+  <si>
+    <t>fada.species-Comments</t>
+  </si>
+  <si>
+    <t>fada.synonyms</t>
+  </si>
+  <si>
+    <t>fada.synonyms-Comments</t>
+  </si>
+  <si>
+    <t>fada.regions_species</t>
+  </si>
+  <si>
+    <t>fada.regions_species-Comments</t>
+  </si>
+  <si>
+    <t>fada.greferences</t>
+  </si>
+  <si>
+    <t>fada.greferences-Comments</t>
+  </si>
+  <si>
+    <t>fada.publications</t>
+  </si>
+  <si>
+    <t>fada.publications-Comments</t>
+  </si>
+  <si>
+    <t>Overall_comments</t>
+  </si>
+  <si>
+    <t>taxonID</t>
+  </si>
+  <si>
+    <t>add provider taxonID to taxons table?</t>
+  </si>
+  <si>
+    <t>species_id</t>
+  </si>
+  <si>
+    <t>refers to id used in the species table</t>
+  </si>
+  <si>
+    <t>scientificNameID</t>
+  </si>
+  <si>
+    <t>acceptedNameUsageID</t>
+  </si>
+  <si>
+    <t>refers to id of accepted name stored in taxons_table</t>
+  </si>
+  <si>
+    <t>parentNameUsageID</t>
+  </si>
+  <si>
+    <t>scientificName</t>
+  </si>
+  <si>
+    <t>Full scientific name including authorship, for xls-files this is currently a concatenation of the following fields: Genus+" " if provided "("+Subgenus+")"+ " "+Species+" "if applicable+Subspecies+" "if Original genus is provided (parenthesis are "Y")"("+Author(s)+" "+Date+if Original genus is provided (parenthesis are "Y")")"</t>
+  </si>
+  <si>
+    <t>Cannonical species name (withouth authorship info!), for xls-files this is currently a concatenation of the following fields: Original genus [Synonym]+" "+ Species/Subspecies [Synonym] OR if synonym for a genus Genus/Subgenus [Synonym]</t>
+  </si>
+  <si>
+    <t>Inclusion of species group (for species table) to be decided!!</t>
+  </si>
+  <si>
+    <t>acceptedNameUsage</t>
+  </si>
+  <si>
+    <t>Not stored as such, field could be used to confirm correct matching with accepted name</t>
+  </si>
+  <si>
+    <t>originalNameUsage</t>
+  </si>
+  <si>
+    <t>content to be parsed</t>
+  </si>
+  <si>
+    <t>original_genus_id, declension_species_id</t>
+  </si>
+  <si>
+    <t>refers to ids stored in taxons table</t>
+  </si>
+  <si>
+    <t>Potentially the originalNames are declared separately in the DwC-A-files, with taxonomicStatus="homotypic synonym"</t>
+  </si>
+  <si>
+    <t>parentNameUsage</t>
+  </si>
+  <si>
+    <t>Not stored as such, field could be used to confirm correct matching with parent</t>
+  </si>
+  <si>
+    <t>namePublishedInID</t>
+  </si>
+  <si>
+    <t>not sure if can be mapped / translate to "ref key"?</t>
+  </si>
+  <si>
+    <t>if record represents a synonym name</t>
+  </si>
+  <si>
+    <t>refkey</t>
+  </si>
+  <si>
+    <t>namePublishedIn</t>
+  </si>
+  <si>
+    <t>[To be checked] Realistic to parse this into the publications table, otherwise add full citation field there for references coming from DwC-A imported groups  - taxons.publication_id</t>
+  </si>
+  <si>
+    <t>namePublishedInYear</t>
+  </si>
+  <si>
+    <t>Not necessarily provided, if this is the case, it should correspond to year in the scientificNameAuthorship field</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>check with entries present/store together with corresponding rank_id; in principle this information is obtained from Catalogue of Life</t>
+  </si>
+  <si>
+    <t>phylum</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>check with entries present/store together with corresponding rank_id</t>
+  </si>
+  <si>
+    <t>Subfamily</t>
+  </si>
+  <si>
+    <t>Tribe</t>
+  </si>
+  <si>
+    <t>Subtribe</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>genus_taxon_id</t>
+  </si>
+  <si>
+    <t>subgenus</t>
+  </si>
+  <si>
+    <t>subgenus_taxon_id</t>
+  </si>
+  <si>
+    <t>Species group</t>
+  </si>
+  <si>
+    <t>species_group_taxon_id</t>
+  </si>
+  <si>
+    <t>to be added to the species table</t>
+  </si>
+  <si>
+    <t>specificEpithet</t>
+  </si>
+  <si>
+    <t>species_taxon_id</t>
+  </si>
+  <si>
+    <t>infraspecificEpithet</t>
+  </si>
+  <si>
+    <t>subspecies_taxon_id</t>
+  </si>
+  <si>
+    <t>taxonRank</t>
+  </si>
+  <si>
+    <t>rank_id</t>
+  </si>
+  <si>
+    <t>translate taxonRank in corresponding rank_id, determine rank based on lowest taxon field filled for xls</t>
+  </si>
+  <si>
+    <t>author names stored in the authors table</t>
+  </si>
+  <si>
+    <t>Parentheses (Y/N)</t>
+  </si>
+  <si>
+    <t>Info used for generating concatenated scientific_name</t>
+  </si>
+  <si>
+    <t>not stored as such, can be derived from presence of Original genus</t>
+  </si>
+  <si>
+    <t>scientificNameAuthorship</t>
+  </si>
+  <si>
+    <t>author_id, year</t>
+  </si>
+  <si>
+    <t>field needs to be parsed</t>
+  </si>
+  <si>
+    <t>nomenclaturalCode</t>
+  </si>
+  <si>
+    <t>taxonomicStatus</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>Only valid/accepted species (status_id=1) stored in the species table, info from DwC-records with taxonomicStatus="homotypic synonym" need to be stored in the original_genus(_id) and if applicable declension_species(_id) fields</t>
+  </si>
+  <si>
+    <t>Field used to determine which names to store in the synonyms table</t>
+  </si>
+  <si>
+    <t>In DwC-AquaRES_field_selection-withPFADA_mapping-v1.1: Not mapped as such, used to establish where/how a record should be stored for rank =&lt; species; IF accepted &gt; species table, IF homotypic synonym &gt; original_genus_id and declension_species_id in corresponding species record in the species table, IF invalid &gt; synonyms table, IF misapplied &gt; [to be discussed] not to be stored or in synonyms table with a specific status flag?</t>
+  </si>
+  <si>
+    <t>Original genus</t>
+  </si>
+  <si>
+    <t>check with entries present/store together with corresponding rank_id, no need to link with higher taxons</t>
+  </si>
+  <si>
+    <t>original_genus_id</t>
+  </si>
+  <si>
+    <t>Original species name</t>
+  </si>
+  <si>
+    <t>declension_species_id</t>
+  </si>
+  <si>
+    <t>This field is also called declension species, if this field is empty the original name is Original genus + species/specificEpithet (of the accepted name)</t>
+  </si>
+  <si>
+    <t>Genus/Subgenus [Synonym]</t>
+  </si>
+  <si>
+    <t>Species/Subspecies [Synonym]</t>
+  </si>
+  <si>
+    <t>Author(s)  [Synonym]</t>
+  </si>
+  <si>
+    <t>for synonym records, author names stored in the authors table</t>
+  </si>
+  <si>
+    <t>for synonym records</t>
+  </si>
+  <si>
+    <t>Original genus [Synonym]</t>
+  </si>
+  <si>
+    <t>only used to generate  genus_species_name</t>
+  </si>
+  <si>
+    <t>field to be added</t>
+  </si>
+  <si>
+    <t>&gt;&gt; groups.metadata table</t>
+  </si>
+  <si>
+    <t>Considered as citation for the dataset. Mapping to groups.metadata</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>[To be checked] Realistic to parse this into the publications table, otherwise add full citation field there for references coming from DwC-A imported groups - taxons.publication_id</t>
+  </si>
+  <si>
+    <t>accessRights</t>
+  </si>
+  <si>
+    <t>&gt;&gt; groups.acces_rights</t>
+  </si>
+  <si>
+    <t>rights</t>
+  </si>
+  <si>
+    <t>&gt;&gt; groups.rights</t>
+  </si>
+  <si>
+    <t>rightsHolder</t>
+  </si>
+  <si>
+    <t>&gt;&gt; groups.rights_holder</t>
+  </si>
+  <si>
+    <t>for FADA, currently considered as users.familyname + users.givenname + groups.coeditors, but probably safer to add new field to groups table</t>
+  </si>
+  <si>
+    <t>datasetID</t>
+  </si>
+  <si>
+    <t>&gt;&gt; provider_dataset_id</t>
+  </si>
+  <si>
+    <t>New field to be added to groups table?</t>
+  </si>
+  <si>
+    <t>datasetName</t>
+  </si>
+  <si>
+    <t>&gt;&gt; groups.dataset_name</t>
+  </si>
+  <si>
+    <t>New field to be added to groups table? For full name rather than name of organism group?</t>
+  </si>
+  <si>
+    <t>Taxonomic comments</t>
+  </si>
+  <si>
+    <t>taxonRemarks</t>
+  </si>
+  <si>
+    <t>taxonomic_comment</t>
+  </si>
+  <si>
+    <t>syn_taxonomic_comment</t>
+  </si>
+  <si>
+    <t>for records representing synonym names</t>
+  </si>
+  <si>
+    <t>Note that comments are not stored for other taxonomic levels using this approach, should we review it?</t>
+  </si>
+  <si>
+    <t>isMarine</t>
+  </si>
+  <si>
+    <t>marine</t>
+  </si>
+  <si>
+    <t>isFreshwater</t>
+  </si>
+  <si>
+    <t>freshwater</t>
+  </si>
+  <si>
+    <t>isTerrestrial</t>
+  </si>
+  <si>
+    <t>terrestrial</t>
+  </si>
+  <si>
+    <t>isBrackish</t>
+  </si>
+  <si>
+    <t>brakish</t>
+  </si>
+  <si>
+    <t>isExtinct</t>
+  </si>
+  <si>
+    <t>extinct</t>
+  </si>
+  <si>
+    <t>lentic?</t>
+  </si>
+  <si>
+    <t>lentic</t>
+  </si>
+  <si>
+    <t>lotic?</t>
+  </si>
+  <si>
+    <t>lotic</t>
+  </si>
+  <si>
+    <t>bodyMass</t>
+  </si>
+  <si>
+    <t>body_mass</t>
+  </si>
+  <si>
+    <t>Parasitic</t>
+  </si>
+  <si>
+    <t>parasitic</t>
+  </si>
+  <si>
+    <t>Aquatic/water dependant</t>
+  </si>
+  <si>
+    <t>aquatic_wd</t>
+  </si>
+  <si>
+    <t>Aquatic/water dependant- subcategory</t>
+  </si>
+  <si>
+    <t>aquatic_wd_subcategory</t>
+  </si>
+  <si>
+    <t>locationID</t>
+  </si>
+  <si>
+    <t>provider_region_id</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>stored as code, PA=8</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>stored as code, AT=1</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>stored as code, AU=3</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>stored as code, OL=6</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>stored as code, NA=4</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>stored as code, NT=5</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>stored as code, ANT=2</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>stored as code, PAC=7</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>fada.regions.name</t>
+  </si>
+  <si>
+    <t>Store names in regions table?</t>
+  </si>
+  <si>
+    <t>TDWG 3rd level codes, separated by comma</t>
+  </si>
+  <si>
+    <t>countryCode</t>
+  </si>
+  <si>
+    <t>fada.regions.code</t>
+  </si>
+  <si>
+    <t>Store code in regions table?</t>
+  </si>
+  <si>
+    <t>exotic</t>
+  </si>
+  <si>
+    <t>occurrenceStatus</t>
+  </si>
+  <si>
+    <t>occurrence_status</t>
+  </si>
+  <si>
+    <t>establishmentMeans</t>
+  </si>
+  <si>
+    <t>establishement_means</t>
+  </si>
+  <si>
+    <t>startDayOfYear</t>
+  </si>
+  <si>
+    <t>endDayOfYear</t>
+  </si>
+  <si>
+    <t>fada.region_species.publication_id / fada.region_species.source_id</t>
+  </si>
+  <si>
+    <t>Fine distribution</t>
+  </si>
+  <si>
+    <t>occurrenceRemarks</t>
+  </si>
+  <si>
+    <t>faunistic_comment</t>
+  </si>
+  <si>
+    <t>Ok here or move to fada.regions_species?</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>provider_id</t>
+  </si>
+  <si>
+    <t>New field to be added for storing original ref key?</t>
+  </si>
+  <si>
+    <t>bibliographic_citation</t>
+  </si>
+  <si>
+    <t>New field to be added for storing full citation</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>publisherlocation</t>
+  </si>
+  <si>
+    <t>sereditor</t>
+  </si>
+  <si>
+    <t>sertitle</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>In this case source includes details such as volume, issue, pages,… as appropriate</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>conservation_id</t>
+  </si>
+  <si>
+    <t>By default set to 9 = Non evaluated</t>
+  </si>
+  <si>
+    <t>In general no info is provided, if the sheet is empty, set value to 9 otherwise interpret data based on conservations table (code field) -&gt; example file: Mammalia</t>
+  </si>
+  <si>
+    <t>CRITERIA 1</t>
+  </si>
+  <si>
+    <t>CRITERIA 2</t>
+  </si>
+  <si>
+    <t>conservation_comment</t>
+  </si>
+  <si>
+    <t>Currently null for all db entries - Field is not mapped to any of the columns of the xls-template: ignore</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>isPreferredName</t>
+  </si>
+  <si>
+    <t>ignore, only used for processing</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>name of source file, not sure why specifically stored here (and not in groups table)</t>
+  </si>
+  <si>
+    <t>row_id</t>
+  </si>
+  <si>
+    <t>Not stored in db, Only non-extinct species names to be saved in FADA database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="12"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="1"/>
+      <i/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="12"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
-      <strike val="0"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -216,139 +893,391 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R125"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScale="80" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85619" customWidth="1"/>
-    <col min="2" max="2" width="13.28492" customWidth="1"/>
-    <col min="3" max="3" width="11.85643" customWidth="1"/>
-    <col min="4" max="4" width="30.71244" customWidth="1"/>
-    <col min="5" max="5" width="21.57013" customWidth="1"/>
-    <col min="6" max="6" width="9.142308"/>
-    <col min="7" max="7" width="20.83203" customWidth="1"/>
-    <col min="8" max="8" width="10.83203" customWidth="1"/>
-    <col min="9" max="9" width="20.83203" customWidth="1"/>
-    <col min="10" max="10" width="10.83203" customWidth="1"/>
-    <col min="11" max="11" width="20.83203" customWidth="1"/>
-    <col min="12" max="12" width="10.83203" customWidth="1"/>
-    <col min="13" max="13" width="20.83203" customWidth="1"/>
-    <col min="14" max="14" width="10.83203" customWidth="1"/>
-    <col min="15" max="15" width="20.83203" customWidth="1"/>
-    <col min="16" max="16" width="10.83203" customWidth="1"/>
-    <col min="17" max="17" width="20.83203" customWidth="1"/>
-    <col min="18" max="18" width="9.142308"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="1" t="str">
-        <v>xls-order</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>xls-sheet</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <v>xls-field</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <v>DwC-Core_or_Extension</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <v>DwC-Term_name</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <v>fada.taxons</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <v>fada.taxons-Comments</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <v>fada.species</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <v>fada.species-Comments</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <v>fada.synonyms</v>
-      </c>
-      <c r="K1" s="1" t="str">
-        <v>fada.synonyms-Comments</v>
-      </c>
-      <c r="L1" s="1" t="str">
-        <v>fada.regions_species</v>
-      </c>
-      <c r="M1" s="1" t="str">
-        <v>fada.regions_species-Comments</v>
-      </c>
-      <c r="N1" s="1" t="str">
-        <v>fada.greferences</v>
-      </c>
-      <c r="O1" s="1" t="str">
-        <v>fada.greferences-Comments</v>
-      </c>
-      <c r="P1" s="2" t="str">
-        <v>fada.publications</v>
-      </c>
-      <c r="Q1" s="2" t="str">
-        <v>fada.publications-Comments</v>
-      </c>
-      <c r="R1" s="1" t="str">
-        <v>Overall_comments</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -380,29 +1309,29 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="str">
-        <v>taxonID</v>
+      <c r="E3" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="3" t="str">
-        <v>add provider taxonID to taxons table?</v>
+      <c r="G3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="3" t="str">
-        <v>species_id</v>
-      </c>
-      <c r="M3" s="3" t="str">
-        <v>refers to id used in the species table</v>
+      <c r="L3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -410,15 +1339,15 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="str">
-        <v>scientificNameID</v>
+      <c r="E4" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -436,15 +1365,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="str">
-        <v>acceptedNameUsageID</v>
+      <c r="E5" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -453,8 +1382,8 @@
       <c r="J5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="3" t="str">
-        <v>refers to id of accepted name stored in taxons_table</v>
+      <c r="K5" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -464,15 +1393,15 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="str">
-        <v>parentNameUsageID</v>
+      <c r="E6" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>5</v>
@@ -490,29 +1419,29 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="str">
-        <v>scientificName</v>
+      <c r="E7" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3" t="str">
-        <v>Full scientific name including authorship, for xls-files this is currently a concatenation of the following fields: Genus+" " if provided "("+Subgenus+")"+ " "+Species+" "if applicable+Subspecies+" "if Original genus is provided (parenthesis are "Y")"("+Author(s)+" "+Date+if Original genus is provided (parenthesis are "Y")")"</v>
+      <c r="I7" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="2" t="str">
-        <v>Cannonical species name (withouth authorship info!), for xls-files this is currently a concatenation of the following fields: Original genus [Synonym]+" "+ Species/Subspecies [Synonym] OR if synonym for a genus Genus/Subgenus [Synonym]</v>
+      <c r="K7" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -520,19 +1449,19 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="2" t="str">
-        <v>Inclusion of species group (for species table) to be decided!!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="str">
-        <v>acceptedNameUsage</v>
+      <c r="E8" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -541,8 +1470,8 @@
       <c r="J8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="3" t="str">
-        <v>Not stored as such, field could be used to confirm correct matching with accepted name</v>
+      <c r="K8" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -552,27 +1481,27 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="1" t="str">
-        <v>originalNameUsage</v>
+      <c r="E9" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="3" t="str">
-        <v>content to be parsed</v>
-      </c>
-      <c r="H9" s="3" t="str">
-        <v>original_genus_id, declension_species_id</v>
-      </c>
-      <c r="I9" s="3" t="str">
-        <v>refers to ids stored in taxons table</v>
+      <c r="G9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -582,25 +1511,25 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="2" t="str">
-        <v>Potentially the originalNames are declared separately in the DwC-A-files, with taxonomicStatus="homotypic synonym"</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="str">
-        <v>parentNameUsage</v>
+      <c r="E10" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="3" t="str">
-        <v>Not stored as such, field could be used to confirm correct matching with parent</v>
+      <c r="G10" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -614,15 +1543,15 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="1" t="str">
-        <v>namePublishedInID</v>
+      <c r="E11" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>9</v>
@@ -640,11 +1569,11 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="3" t="str">
-        <v>not sure if can be mapped / translate to "ref key"?</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="R11" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -667,13 +1596,13 @@
       <c r="J12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="3" t="str">
-        <v>if record represents a synonym name</v>
+      <c r="K12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="3" t="str">
-        <v>refkey</v>
+      <c r="N12" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>13</v>
@@ -682,21 +1611,21 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="str">
-        <v>namePublishedIn</v>
+      <c r="E13" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="str">
-        <v>[To be checked] Realistic to parse this into the publications table, otherwise add full citation field there for references coming from DwC-A imported groups  - taxons.publication_id</v>
+      <c r="G13" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -710,21 +1639,21 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="1" t="str">
-        <v>namePublishedInYear</v>
+      <c r="E14" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="3" t="str">
-        <v>Not necessarily provided, if this is the case, it should correspond to year in the scientificNameAuthorship field</v>
+      <c r="G14" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -738,7 +1667,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -770,21 +1699,21 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="str">
-        <v>kingdom</v>
+      <c r="E16" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="3" t="str">
-        <v>check with entries present/store together with corresponding rank_id; in principle this information is obtained from Catalogue of Life</v>
+      <c r="G16" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -798,15 +1727,15 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="1" t="str">
-        <v>phylum</v>
+      <c r="E17" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>18</v>
@@ -824,15 +1753,15 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="1" t="str">
-        <v>class</v>
+      <c r="E18" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>18</v>
@@ -850,15 +1779,15 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="1" t="str">
-        <v>order</v>
+      <c r="E19" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>18</v>
@@ -876,27 +1805,27 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1" t="str">
-        <v>Family</v>
+      <c r="C20" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="1" t="str">
-        <v>family</v>
+      <c r="E20" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="5" t="str">
-        <v>check with entries present/store together with corresponding rank_id</v>
+      <c r="G20" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -910,15 +1839,15 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="1" t="str">
-        <v>Subfamily</v>
+      <c r="C21" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -938,15 +1867,15 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="str">
-        <v>Tribe</v>
+      <c r="C22" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -966,15 +1895,15 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="1" t="str">
-        <v>Subtribe</v>
+      <c r="C23" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -994,7 +1923,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>5</v>
       </c>
@@ -1007,15 +1936,15 @@
       <c r="D24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="1" t="str">
-        <v>genus</v>
+      <c r="E24" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="3" t="str">
-        <v>genus_taxon_id</v>
+      <c r="H24" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>20</v>
@@ -1030,7 +1959,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>6</v>
       </c>
@@ -1043,15 +1972,15 @@
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="1" t="str">
-        <v>subgenus</v>
+      <c r="E25" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="3" t="str">
-        <v>subgenus_taxon_id</v>
+      <c r="H25" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>20</v>
@@ -1066,15 +1995,15 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="1" t="str">
-        <v>Species group</v>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1082,11 +2011,11 @@
         <v>18</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="2" t="str">
-        <v>species_group_taxon_id</v>
-      </c>
-      <c r="I26" s="2" t="str">
-        <v>to be added to the species table</v>
+      <c r="H26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1098,7 +2027,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>8</v>
       </c>
@@ -1111,15 +2040,15 @@
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="1" t="str">
-        <v>specificEpithet</v>
+      <c r="E27" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="3" t="str">
-        <v>species_taxon_id</v>
+      <c r="H27" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>20</v>
@@ -1134,7 +2063,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>9</v>
       </c>
@@ -1147,15 +2076,15 @@
       <c r="D28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="1" t="str">
-        <v>infraspecificEpithet</v>
+      <c r="E28" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="3" t="str">
-        <v>subspecies_taxon_id</v>
+      <c r="H28" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>20</v>
@@ -1170,21 +2099,21 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="1" t="str">
-        <v>taxonRank</v>
-      </c>
-      <c r="F29" s="3" t="str">
-        <v>rank_id</v>
-      </c>
-      <c r="G29" s="3" t="str">
-        <v>translate taxonRank in corresponding rank_id, determine rank based on lowest taxon field filled for xls</v>
+      <c r="E29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1198,7 +2127,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -1213,8 +2142,8 @@
       <c r="F30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="3" t="str">
-        <v>author names stored in the authors table</v>
+      <c r="G30" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1228,7 +2157,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>11</v>
       </c>
@@ -1256,15 +2185,15 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="1" t="str">
-        <v>Parentheses (Y/N)</v>
+      <c r="C32" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1273,8 +2202,8 @@
       <c r="H32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="3" t="str">
-        <v>Info used for generating concatenated scientific_name</v>
+      <c r="I32" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1284,25 +2213,25 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="1" t="str">
-        <v>not stored as such, can be derived from presence of Original genus</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="R32" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="1" t="str">
-        <v>scientificNameAuthorship</v>
-      </c>
-      <c r="F33" s="3" t="str">
-        <v>author_id, year</v>
-      </c>
-      <c r="G33" s="3" t="str">
-        <v>field needs to be parsed</v>
+      <c r="E33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1316,15 +2245,15 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="4" t="str">
-        <v>nomenclaturalCode</v>
+      <c r="E34" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1342,27 +2271,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="1" t="str">
-        <v>taxonomicStatus</v>
+      <c r="E35" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="3" t="str">
-        <v>status_id</v>
-      </c>
-      <c r="I35" s="3" t="str">
-        <v>Only valid/accepted species (status_id=1) stored in the species table, info from DwC-records with taxonomicStatus="homotypic synonym" need to be stored in the original_genus(_id) and if applicable declension_species(_id) fields</v>
+      <c r="H35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="J35" s="1"/>
-      <c r="K35" s="3" t="str">
-        <v>Field used to determine which names to store in the synonyms table</v>
+      <c r="K35" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -1370,30 +2299,30 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1" t="str">
-        <v>In DwC-AquaRES_field_selection-withPFADA_mapping-v1.1: Not mapped as such, used to establish where/how a record should be stored for rank =&lt; species; IF accepted &gt; species table, IF homotypic synonym &gt; original_genus_id and declension_species_id in corresponding species record in the species table, IF invalid &gt; synonyms table, IF misapplied &gt; [to be discussed] not to be stored or in synonyms table with a specific status flag?</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="R35" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="1" t="str">
-        <v>Original genus</v>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="5" t="str">
-        <v>check with entries present/store together with corresponding rank_id, no need to link with higher taxons</v>
-      </c>
-      <c r="H36" s="3" t="str">
-        <v>original_genus_id</v>
+      <c r="G36" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>20</v>
@@ -1408,15 +2337,15 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="1" t="str">
-        <v>Original species name</v>
+      <c r="C37" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1424,8 +2353,8 @@
         <v>18</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="3" t="str">
-        <v>declension_species_id</v>
+      <c r="H37" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>20</v>
@@ -1438,19 +2367,19 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1" t="str">
-        <v>This field is also called declension species, if this field is empty the original name is Original genus + species/specificEpithet (of the accepted name)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="R37" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="1" t="str">
-        <v>Genus/Subgenus [Synonym]</v>
+      <c r="C38" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1474,15 +2403,15 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="1" t="str">
-        <v>Species/Subspecies [Synonym]</v>
+      <c r="C39" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1506,23 +2435,23 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="1" t="str">
-        <v>Author(s)  [Synonym]</v>
+      <c r="C40" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="3" t="str">
-        <v>for synonym records, author names stored in the authors table</v>
+      <c r="G40" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -1536,7 +2465,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>18</v>
       </c>
@@ -1551,8 +2480,8 @@
       <c r="F41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="3" t="str">
-        <v>for synonym records</v>
+      <c r="G41" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -1566,15 +2495,15 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>19</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="1" t="str">
-        <v>Original genus [Synonym]</v>
+      <c r="C42" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1585,8 +2514,8 @@
       <c r="J42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K42" s="3" t="str">
-        <v>only used to generate  genus_species_name</v>
+      <c r="K42" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -1596,7 +2525,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1609,8 +2538,8 @@
       <c r="F43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="2" t="str">
-        <v>field to be added</v>
+      <c r="G43" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -1624,7 +2553,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1634,11 +2563,11 @@
       <c r="E44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="2" t="str">
-        <v>&gt;&gt; groups.metadata table</v>
-      </c>
-      <c r="G44" s="2" t="str">
-        <v>Considered as citation for the dataset. Mapping to groups.metadata</v>
+      <c r="F44" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1652,21 +2581,21 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="1" t="str">
-        <v>references</v>
+      <c r="E45" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="2" t="str">
-        <v>[To be checked] Realistic to parse this into the publications table, otherwise add full citation field there for references coming from DwC-A imported groups - taxons.publication_id</v>
+      <c r="G45" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1680,18 +2609,18 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E46" s="1" t="str">
-        <v>accessRights</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <v>&gt;&gt; groups.acces_rights</v>
+      <c r="E46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>30</v>
@@ -1708,18 +2637,18 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="1" t="str">
-        <v>rights</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <v>&gt;&gt; groups.rights</v>
+      <c r="E47" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>30</v>
@@ -1736,21 +2665,21 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E48" s="1" t="str">
-        <v>rightsHolder</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <v>&gt;&gt; groups.rights_holder</v>
-      </c>
-      <c r="G48" s="2" t="str">
-        <v>for FADA, currently considered as users.familyname + users.givenname + groups.coeditors, but probably safer to add new field to groups table</v>
+      <c r="E48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -1764,21 +2693,21 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="1" t="str">
-        <v>datasetID</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <v>&gt;&gt; provider_dataset_id</v>
-      </c>
-      <c r="G49" s="2" t="str">
-        <v>New field to be added to groups table?</v>
+      <c r="E49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1792,21 +2721,21 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="1" t="str">
-        <v>datasetName</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <v>&gt;&gt; groups.dataset_name</v>
-      </c>
-      <c r="G50" s="2" t="str">
-        <v>New field to be added to groups table? For full name rather than name of organism group?</v>
+      <c r="E50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1820,33 +2749,33 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="1" t="str">
-        <v>Taxonomic comments</v>
+      <c r="C51" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="1" t="str">
-        <v>taxonRemarks</v>
+      <c r="E51" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="5" t="str">
-        <v>taxonomic_comment</v>
+      <c r="H51" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="I51" s="1"/>
-      <c r="J51" s="3" t="str">
-        <v>syn_taxonomic_comment</v>
-      </c>
-      <c r="K51" s="3" t="str">
-        <v>for records representing synonym names</v>
+      <c r="J51" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -1854,11 +2783,11 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
-      <c r="R51" s="2" t="str">
-        <v>Note that comments are not stored for other taxonomic levels using this approach, should we review it?</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="R51" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1882,7 +2811,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -1908,7 +2837,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2</v>
       </c>
@@ -1934,7 +2863,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3</v>
       </c>
@@ -1960,7 +2889,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>4</v>
       </c>
@@ -1986,7 +2915,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>5</v>
       </c>
@@ -2012,7 +2941,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>6</v>
       </c>
@@ -2038,20 +2967,22 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18">
-      <c r="A59" s="1"/>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>25</v>
+      </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E59" s="1" t="str">
-        <v>isMarine</v>
+      <c r="E59" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="2" t="str">
-        <v>marine</v>
+      <c r="H59" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>34</v>
@@ -2066,20 +2997,22 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18">
-      <c r="A60" s="1"/>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>26</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E60" s="1" t="str">
-        <v>isFreshwater</v>
+      <c r="E60" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="2" t="str">
-        <v>freshwater</v>
+      <c r="H60" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>34</v>
@@ -2094,20 +3027,22 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18">
-      <c r="A61" s="1"/>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>27</v>
+      </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E61" s="1" t="str">
-        <v>isTerrestrial</v>
+      <c r="E61" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="2" t="str">
-        <v>terrestrial</v>
+      <c r="H61" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>34</v>
@@ -2122,20 +3057,22 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18">
-      <c r="A62" s="1"/>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>28</v>
+      </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E62" s="1" t="str">
-        <v>isBrackish</v>
+      <c r="E62" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="2" t="str">
-        <v>brakish</v>
+      <c r="H62" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>34</v>
@@ -2150,23 +3087,23 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E63" s="1" t="str">
-        <v>isExtinct</v>
+      <c r="E63" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="2" t="str">
-        <v>extinct</v>
+      <c r="H63" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>34</v>
+        <v>267</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -2178,22 +3115,22 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C64" s="1" t="str">
-        <v>lentic?</v>
+      <c r="C64" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="2" t="str">
-        <v>lentic</v>
+      <c r="H64" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>34</v>
@@ -2208,22 +3145,22 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="1" t="str">
-        <v>lotic?</v>
+      <c r="C65" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="2" t="str">
-        <v>lotic</v>
+      <c r="H65" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>34</v>
@@ -2238,22 +3175,22 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>21</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C66" s="1" t="str">
-        <v>bodyMass</v>
+      <c r="C66" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="2" t="str">
-        <v>body_mass</v>
+      <c r="H66" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>34</v>
@@ -2268,22 +3205,22 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>22</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="1" t="str">
-        <v>Parasitic</v>
+      <c r="C67" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="2" t="str">
-        <v>parasitic</v>
+      <c r="H67" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>34</v>
@@ -2298,22 +3235,22 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>23</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="1" t="str">
-        <v>Aquatic/water dependant</v>
+      <c r="C68" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="2" t="str">
-        <v>aquatic_wd</v>
+      <c r="H68" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>34</v>
@@ -2328,22 +3265,22 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C69" s="1" t="str">
-        <v>Aquatic/water dependant- subcategory</v>
+      <c r="C69" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="H69" s="2" t="str">
-        <v>aquatic_wd_subcategory</v>
+      <c r="H69" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>34</v>
@@ -2358,7 +3295,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2382,15 +3319,15 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E71" s="1" t="str">
-        <v>locationID</v>
+      <c r="E71" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2398,8 +3335,8 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="2" t="str">
-        <v>provider_region_id</v>
+      <c r="L71" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>36</v>
@@ -2410,15 +3347,15 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>7</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C72" s="1" t="str">
-        <v>PA</v>
+      <c r="C72" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2431,8 +3368,8 @@
       <c r="L72" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M72" s="3" t="str">
-        <v>stored as code, PA=8</v>
+      <c r="M72" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -2440,15 +3377,15 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C73" s="1" t="str">
-        <v>AT</v>
+      <c r="C73" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2461,8 +3398,8 @@
       <c r="L73" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M73" s="3" t="str">
-        <v>stored as code, AT=1</v>
+      <c r="M73" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -2470,15 +3407,15 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>9</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C74" s="1" t="str">
-        <v>AU</v>
+      <c r="C74" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2491,8 +3428,8 @@
       <c r="L74" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M74" s="3" t="str">
-        <v>stored as code, AU=3</v>
+      <c r="M74" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -2500,15 +3437,15 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>10</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C75" s="1" t="str">
-        <v>OL</v>
+      <c r="C75" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -2521,8 +3458,8 @@
       <c r="L75" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M75" s="3" t="str">
-        <v>stored as code, OL=6</v>
+      <c r="M75" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -2530,15 +3467,15 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>11</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C76" s="1" t="str">
-        <v>NA</v>
+      <c r="C76" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -2551,8 +3488,8 @@
       <c r="L76" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M76" s="3" t="str">
-        <v>stored as code, NA=4</v>
+      <c r="M76" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -2560,15 +3497,15 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>12</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="1" t="str">
-        <v>NT</v>
+      <c r="C77" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2581,8 +3518,8 @@
       <c r="L77" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M77" s="3" t="str">
-        <v>stored as code, NT=5</v>
+      <c r="M77" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -2590,15 +3527,15 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>13</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C78" s="1" t="str">
-        <v>ANT</v>
+      <c r="C78" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2611,8 +3548,8 @@
       <c r="L78" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M78" s="3" t="str">
-        <v>stored as code, ANT=2</v>
+      <c r="M78" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -2620,15 +3557,15 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>14</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C79" s="1" t="str">
-        <v>PAC</v>
+      <c r="C79" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -2641,8 +3578,8 @@
       <c r="L79" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M79" s="3" t="str">
-        <v>stored as code, PAC=7</v>
+      <c r="M79" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -2650,15 +3587,15 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E80" s="1" t="str">
-        <v>locality</v>
+      <c r="E80" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -2666,11 +3603,11 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
-      <c r="L80" s="3" t="str">
-        <v>fada.regions.name</v>
-      </c>
-      <c r="M80" s="3" t="str">
-        <v>Store names in regions table?</v>
+      <c r="L80" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="M80" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -2678,21 +3615,21 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>16</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C81" s="1" t="str">
-        <v>TDWG 3rd level codes, separated by comma</v>
+      <c r="C81" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E81" s="1" t="str">
-        <v>countryCode</v>
+      <c r="E81" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -2700,11 +3637,11 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
-      <c r="L81" s="3" t="str">
-        <v>fada.regions.code</v>
-      </c>
-      <c r="M81" s="3" t="str">
-        <v>Store code in regions table?</v>
+      <c r="L81" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="M81" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -2712,26 +3649,26 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>20</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="1" t="str">
-        <v>exotic</v>
+      <c r="C82" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E82" s="1" t="str">
-        <v>occurrenceStatus</v>
+      <c r="E82" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="2" t="str">
-        <v>occurrence_status</v>
+      <c r="H82" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>34</v>
@@ -2746,20 +3683,20 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E83" s="1" t="str">
-        <v>establishmentMeans</v>
+      <c r="E83" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="2" t="str">
-        <v>establishement_means</v>
+      <c r="H83" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>34</v>
@@ -2774,15 +3711,15 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E84" s="4" t="str">
-        <v>startDayOfYear</v>
+      <c r="E84" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -2800,15 +3737,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E85" s="4" t="str">
-        <v>endDayOfYear</v>
+      <c r="E85" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -2826,7 +3763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>17</v>
       </c>
@@ -2848,8 +3785,8 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
-      <c r="L86" s="2" t="str">
-        <v>fada.region_species.publication_id / fada.region_species.source_id</v>
+      <c r="L86" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="M86" s="2" t="s">
         <v>36</v>
@@ -2860,29 +3797,29 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>15</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="1" t="str">
-        <v>Fine distribution</v>
+      <c r="C87" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E87" s="1" t="str">
-        <v>occurrenceRemarks</v>
+      <c r="E87" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-      <c r="H87" s="2" t="str">
-        <v>faunistic_comment</v>
-      </c>
-      <c r="I87" s="2" t="str">
-        <v>Ok here or move to fada.regions_species?</v>
+      <c r="H87" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -2894,7 +3831,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2918,7 +3855,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>5</v>
       </c>
@@ -2931,8 +3868,8 @@
       <c r="D89" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E89" s="1" t="str">
-        <v>identifier</v>
+      <c r="E89" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -2944,15 +3881,15 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="2" t="str">
-        <v>provider_id</v>
-      </c>
-      <c r="Q89" s="2" t="str">
-        <v>New field to be added for storing original ref key?</v>
+      <c r="P89" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q89" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2972,23 +3909,23 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="2" t="str">
-        <v>bibliographic_citation</v>
-      </c>
-      <c r="Q90" s="2" t="str">
-        <v>New field to be added for storing full citation</v>
+      <c r="P90" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q90" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C91" s="1" t="str">
-        <v>Author</v>
+      <c r="C91" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -3000,8 +3937,8 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
-      <c r="N91" s="5" t="str">
-        <v>author</v>
+      <c r="N91" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="O91" s="1"/>
       <c r="P91" s="3" t="s">
@@ -3010,15 +3947,15 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C92" s="1" t="str">
-        <v>Year</v>
+      <c r="C92" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -3040,15 +3977,15 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>3</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C93" s="1" t="str">
-        <v>Title</v>
+      <c r="C93" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>40</v>
@@ -3074,7 +4011,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3090,13 +4027,13 @@
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
-      <c r="P94" s="2" t="str">
-        <v>publisher</v>
+      <c r="P94" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3112,13 +4049,13 @@
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
-      <c r="P95" s="2" t="str">
-        <v>volume</v>
+      <c r="P95" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3134,13 +4071,13 @@
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
-      <c r="P96" s="2" t="str">
-        <v>issue</v>
+      <c r="P96" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3156,13 +4093,13 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
-      <c r="P97" s="2" t="str">
-        <v>pages</v>
+      <c r="P97" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3178,13 +4115,13 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
-      <c r="P98" s="2" t="str">
-        <v>editor</v>
+      <c r="P98" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3200,13 +4137,13 @@
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
-      <c r="P99" s="2" t="str">
-        <v>publisherlocation</v>
+      <c r="P99" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3222,13 +4159,13 @@
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
-      <c r="P100" s="2" t="str">
-        <v>sereditor</v>
+      <c r="P100" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3244,21 +4181,21 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
-      <c r="P101" s="2" t="str">
-        <v>sertitle</v>
+      <c r="P101" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E102" s="1" t="str">
-        <v>creator</v>
+      <c r="E102" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
@@ -3274,15 +4211,15 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E103" s="1" t="str">
-        <v>date</v>
+      <c r="E103" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -3298,15 +4235,15 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>4</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C104" s="1" t="str">
-        <v>Source</v>
+      <c r="C104" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>40</v>
@@ -3325,8 +4262,8 @@
       <c r="N104" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O104" s="3" t="str">
-        <v>In this case source includes details such as volume, issue, pages,… as appropriate</v>
+      <c r="O104" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="P104" s="3" t="s">
         <v>39</v>
@@ -3334,15 +4271,15 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E105" s="1" t="str">
-        <v>description</v>
+      <c r="E105" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
@@ -3358,15 +4295,15 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E106" s="1" t="str">
-        <v>type</v>
+      <c r="E106" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
@@ -3382,7 +4319,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>6</v>
       </c>
@@ -3412,7 +4349,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>1</v>
       </c>
@@ -3438,7 +4375,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -3464,7 +4401,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>3</v>
       </c>
@@ -3490,7 +4427,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>4</v>
       </c>
@@ -3516,25 +4453,25 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>5</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C112" s="1" t="str">
-        <v>Category</v>
+      <c r="C112" s="1" t="s">
+        <v>251</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
-      <c r="H112" s="3" t="str">
-        <v>conservation_id</v>
-      </c>
-      <c r="I112" s="3" t="str">
-        <v>By default set to 9 = Non evaluated</v>
+      <c r="H112" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -3544,19 +4481,19 @@
       <c r="O112" s="1"/>
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
-      <c r="R112" s="1" t="str">
-        <v>In general no info is provided, if the sheet is empty, set value to 9 otherwise interpret data based on conservations table (code field) -&gt; example file: Mammalia</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18">
+      <c r="R112" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>6</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C113" s="4" t="str">
-        <v>CRITERIA 1</v>
+      <c r="C113" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -3576,15 +4513,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>7</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C114" s="4" t="str">
-        <v>CRITERIA 2</v>
+      <c r="C114" s="4" t="s">
+        <v>256</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -3604,7 +4541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3612,11 +4549,11 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
-      <c r="H115" s="7" t="str">
-        <v>conservation_comment</v>
-      </c>
-      <c r="I115" s="7" t="str">
-        <v>Currently null for all db entries - Field is not mapped to any of the columns of the xls-template: ignore</v>
+      <c r="H115" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
@@ -3630,7 +4567,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3656,7 +4593,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3682,7 +4619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3708,15 +4645,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E119" s="4" t="str">
-        <v>language</v>
+      <c r="E119" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
@@ -3734,15 +4671,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E120" s="4" t="str">
-        <v>isPreferredName</v>
+      <c r="E120" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -3760,7 +4697,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>1</v>
       </c>
@@ -3784,19 +4721,19 @@
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
       <c r="Q121" s="1"/>
-      <c r="R121" s="1" t="str">
-        <v>ignore, only used for processing</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18">
+      <c r="R121" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>2</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C122" s="4" t="str">
-        <v>Description</v>
+      <c r="C122" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -3816,15 +4753,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>3</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C123" s="4" t="str">
-        <v>Comments</v>
+      <c r="C123" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -3844,7 +4781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3858,17 +4795,17 @@
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
-      <c r="N124" s="3" t="str">
-        <v>file_name</v>
-      </c>
-      <c r="O124" s="3" t="str">
-        <v>name of source file, not sure why specifically stored here (and not in groups table)</v>
+      <c r="N124" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="O124" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="P124" s="1"/>
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3882,8 +4819,8 @@
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
-      <c r="N125" s="3" t="str">
-        <v>row_id</v>
+      <c r="N125" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="O125" s="1"/>
       <c r="P125" s="1"/>
@@ -3892,8 +4829,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Field mapping draft update following database changes
Draft update following database changes, remains to be discussed with
Michel
</commit_message>
<xml_diff>
--- a/database-info/Field_mapping.xlsx
+++ b/database-info/Field_mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14440" yWindow="3840" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="980" yWindow="1020" windowWidth="25780" windowHeight="25420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="261">
   <si>
     <t>id</t>
   </si>
@@ -61,9 +61,6 @@
     <t>publication_id</t>
   </si>
   <si>
-    <t>generate id refering to publications table</t>
-  </si>
-  <si>
     <t>Taxonomy</t>
   </si>
   <si>
@@ -133,15 +130,9 @@
     <t>Faunistic</t>
   </si>
   <si>
-    <t>New field in fada.species or in new speciesprofile table?</t>
-  </si>
-  <si>
     <t>Distribution</t>
   </si>
   <si>
-    <t>New field to be added to fada.region_species?</t>
-  </si>
-  <si>
     <t>region_id</t>
   </si>
   <si>
@@ -217,21 +208,12 @@
     <t>fada.greferences-Comments</t>
   </si>
   <si>
-    <t>fada.publications</t>
-  </si>
-  <si>
-    <t>fada.publications-Comments</t>
-  </si>
-  <si>
     <t>Overall_comments</t>
   </si>
   <si>
     <t>taxonID</t>
   </si>
   <si>
-    <t>add provider taxonID to taxons table?</t>
-  </si>
-  <si>
     <t>species_id</t>
   </si>
   <si>
@@ -259,9 +241,6 @@
     <t>Cannonical species name (withouth authorship info!), for xls-files this is currently a concatenation of the following fields: Original genus [Synonym]+" "+ Species/Subspecies [Synonym] OR if synonym for a genus Genus/Subgenus [Synonym]</t>
   </si>
   <si>
-    <t>Inclusion of species group (for species table) to be decided!!</t>
-  </si>
-  <si>
     <t>acceptedNameUsage</t>
   </si>
   <si>
@@ -361,12 +340,6 @@
     <t>Species group</t>
   </si>
   <si>
-    <t>species_group_taxon_id</t>
-  </si>
-  <si>
-    <t>to be added to the species table</t>
-  </si>
-  <si>
     <t>specificEpithet</t>
   </si>
   <si>
@@ -394,12 +367,6 @@
     <t>Parentheses (Y/N)</t>
   </si>
   <si>
-    <t>Info used for generating concatenated scientific_name</t>
-  </si>
-  <si>
-    <t>not stored as such, can be derived from presence of Original genus</t>
-  </si>
-  <si>
     <t>scientificNameAuthorship</t>
   </si>
   <si>
@@ -466,9 +433,6 @@
     <t>only used to generate  genus_species_name</t>
   </si>
   <si>
-    <t>field to be added</t>
-  </si>
-  <si>
     <t>&gt;&gt; groups.metadata table</t>
   </si>
   <si>
@@ -607,9 +571,6 @@
     <t>locationID</t>
   </si>
   <si>
-    <t>provider_region_id</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -661,48 +622,27 @@
     <t>locality</t>
   </si>
   <si>
-    <t>fada.regions.name</t>
-  </si>
-  <si>
-    <t>Store names in regions table?</t>
-  </si>
-  <si>
     <t>TDWG 3rd level codes, separated by comma</t>
   </si>
   <si>
     <t>countryCode</t>
   </si>
   <si>
-    <t>fada.regions.code</t>
-  </si>
-  <si>
-    <t>Store code in regions table?</t>
-  </si>
-  <si>
     <t>exotic</t>
   </si>
   <si>
     <t>occurrenceStatus</t>
   </si>
   <si>
-    <t>occurrence_status</t>
-  </si>
-  <si>
     <t>establishmentMeans</t>
   </si>
   <si>
-    <t>establishement_means</t>
-  </si>
-  <si>
     <t>startDayOfYear</t>
   </si>
   <si>
     <t>endDayOfYear</t>
   </si>
   <si>
-    <t>fada.region_species.publication_id / fada.region_species.source_id</t>
-  </si>
-  <si>
     <t>Fine distribution</t>
   </si>
   <si>
@@ -712,24 +652,9 @@
     <t>faunistic_comment</t>
   </si>
   <si>
-    <t>Ok here or move to fada.regions_species?</t>
-  </si>
-  <si>
     <t>identifier</t>
   </si>
   <si>
-    <t>provider_id</t>
-  </si>
-  <si>
-    <t>New field to be added for storing original ref key?</t>
-  </si>
-  <si>
-    <t>bibliographic_citation</t>
-  </si>
-  <si>
-    <t>New field to be added for storing full citation</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -742,30 +667,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>issue</t>
-  </si>
-  <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>editor</t>
-  </si>
-  <si>
-    <t>publisherlocation</t>
-  </si>
-  <si>
-    <t>sereditor</t>
-  </si>
-  <si>
-    <t>sertitle</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
@@ -832,7 +733,85 @@
     <t>row_id</t>
   </si>
   <si>
-    <t>Not stored in db, Only non-extinct species names to be saved in FADA database</t>
+    <t>add provider taxonID in import schema (not stored in fada schema)</t>
+  </si>
+  <si>
+    <t>Note: species group (taxons with rank_id = 13) is not included in species table nor in generated name</t>
+  </si>
+  <si>
+    <t>greferences.id</t>
+  </si>
+  <si>
+    <t>generate id refering to greferences table</t>
+  </si>
+  <si>
+    <t>&gt;&gt; greferences table?</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Note: species group info not stored in species table</t>
+  </si>
+  <si>
+    <t>parentheses</t>
+  </si>
+  <si>
+    <t>Info stored in new parentheses field and used for generating concatenated scientific_name</t>
+  </si>
+  <si>
+    <t>Note: originally not stored as such, but added during db structure update (incl. generation of content for this field)</t>
+  </si>
+  <si>
+    <t>Not stored as such</t>
+  </si>
+  <si>
+    <t>fada.groups</t>
+  </si>
+  <si>
+    <t>fada.groups-Comments</t>
+  </si>
+  <si>
+    <t>New field in speciesprofile table</t>
+  </si>
+  <si>
+    <t>Not stored in db, used for filtering; Only non-extinct species names to be saved in FADA database</t>
+  </si>
+  <si>
+    <t>regions_all.code</t>
+  </si>
+  <si>
+    <t>Create new entries in fada.regions_all if not found. Specify at least regiontype, code and name.</t>
+  </si>
+  <si>
+    <t>fada.regions_all.name</t>
+  </si>
+  <si>
+    <t>fada.regions_all.code</t>
+  </si>
+  <si>
+    <t>Store code in regions_all table and reference ID in regions_species table</t>
+  </si>
+  <si>
+    <t>Store names in regions_all table and reference ID in regions_species table</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Add link to corresponding greferences.ID to fada.taxons_faunisticreferences</t>
+  </si>
+  <si>
+    <t>greference_id</t>
+  </si>
+  <si>
+    <t>Note: field could be moved to fada.regions_species?</t>
+  </si>
+  <si>
+    <t>Not stored as such for the moment, only included in bibliographicCitation field</t>
+  </si>
+  <si>
+    <t>Name info only used for obtaining species_id</t>
   </si>
 </sst>
 </file>
@@ -869,7 +848,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -891,6 +870,24 @@
         <fgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -901,12 +898,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -915,10 +916,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1194,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R125"/>
+  <dimension ref="A1:R117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD82"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,58 +1232,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -1303,9 +1312,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
@@ -1317,21 +1324,21 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="3" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -1347,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1373,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1383,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1401,7 +1408,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>5</v>
@@ -1427,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1435,13 +1442,13 @@
         <v>6</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1450,7 +1457,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="2" t="s">
-        <v>76</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1461,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1471,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1489,19 +1496,19 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1512,7 +1519,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1523,13 +1530,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1551,13 +1558,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>9</v>
+        <v>79</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1570,7 +1577,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1578,18 +1585,18 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="3" t="s">
-        <v>9</v>
+      <c r="F12" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1597,18 +1604,18 @@
         <v>9</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1619,13 +1626,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>238</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1647,13 +1654,13 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1674,29 +1681,29 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1707,13 +1714,13 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1735,10 +1742,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1761,10 +1768,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1787,10 +1794,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1810,22 +1817,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1844,15 +1851,15 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1872,15 +1879,15 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1900,15 +1907,15 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1928,26 +1935,26 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1964,26 +1971,26 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2000,22 +2007,22 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>111</v>
+      <c r="H26" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>239</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2025,33 +2032,35 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="R26" s="9" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2068,26 +2077,26 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2107,13 +2116,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2132,18 +2141,18 @@
         <v>10</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2162,15 +2171,15 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2190,20 +2199,20 @@
         <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>121</v>
+      <c r="H32" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2214,7 +2223,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1" t="s">
-        <v>122</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -2225,13 +2234,13 @@
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2253,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2279,19 +2288,19 @@
         <v>2</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2300,7 +2309,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -2308,10 +2317,10 @@
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2319,13 +2328,13 @@
         <v>8</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2342,22 +2351,22 @@
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2368,7 +2377,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -2376,15 +2385,15 @@
         <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2393,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2408,15 +2417,15 @@
         <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2425,7 +2434,7 @@
         <v>7</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2440,18 +2449,18 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2470,18 +2479,18 @@
         <v>18</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2500,10 +2509,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2515,7 +2524,7 @@
         <v>7</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2533,13 +2542,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2549,8 +2552,10 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="P43" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q43" s="2"/>
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -2561,13 +2566,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2577,8 +2576,12 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="P44" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="R44" s="1"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
@@ -2589,13 +2592,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2605,8 +2602,12 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="P45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="R45" s="1"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
@@ -2617,13 +2618,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2633,8 +2628,12 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="P46" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="R46" s="1"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -2645,13 +2644,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -2661,8 +2654,12 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="P47" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="R47" s="1"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
@@ -2673,13 +2670,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2689,8 +2680,12 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="P48" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="R48" s="1"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
@@ -2701,13 +2696,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -2717,8 +2706,12 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="P49" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="R49" s="1"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
@@ -2729,13 +2722,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2745,8 +2732,12 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
+      <c r="P50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
@@ -2754,28 +2745,28 @@
         <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="5" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2784,7 +2775,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
@@ -2792,10 +2783,10 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2816,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2842,10 +2833,10 @@
         <v>2</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2868,10 +2859,10 @@
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2894,10 +2885,10 @@
         <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2920,10 +2911,10 @@
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2946,10 +2937,10 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2974,18 +2965,18 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -3004,18 +2995,18 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="2" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
@@ -3034,18 +3025,18 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="2" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -3064,18 +3055,18 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="2" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -3092,18 +3083,18 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="2" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -3120,20 +3111,20 @@
         <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -3150,20 +3141,20 @@
         <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -3180,20 +3171,20 @@
         <v>21</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -3210,20 +3201,20 @@
         <v>22</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -3240,20 +3231,20 @@
         <v>23</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -3270,20 +3261,20 @@
         <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -3300,10 +3291,10 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -3324,10 +3315,10 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3336,10 +3327,10 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="2" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>36</v>
+        <v>250</v>
       </c>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -3352,10 +3343,10 @@
         <v>7</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3366,10 +3357,10 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -3382,10 +3373,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -3396,10 +3387,10 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -3412,10 +3403,10 @@
         <v>9</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -3426,10 +3417,10 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -3442,10 +3433,10 @@
         <v>10</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3456,10 +3447,10 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -3472,10 +3463,10 @@
         <v>11</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -3486,10 +3477,10 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M76" s="3" t="s">
-        <v>202</v>
+        <v>34</v>
+      </c>
+      <c r="M76" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
@@ -3502,10 +3493,10 @@
         <v>12</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3516,10 +3507,10 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
@@ -3532,10 +3523,10 @@
         <v>13</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3546,10 +3537,10 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -3562,10 +3553,10 @@
         <v>14</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3576,10 +3567,10 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -3592,10 +3583,10 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3604,10 +3595,10 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="3" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -3620,16 +3611,16 @@
         <v>16</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3638,10 +3629,10 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="3" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
@@ -3654,24 +3645,24 @@
         <v>20</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>34</v>
+      <c r="H82" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -3681,25 +3672,27 @@
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
+      <c r="R82" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>34</v>
+      <c r="H83" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>239</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -3709,17 +3702,19 @@
       <c r="O83" s="1"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
-      <c r="R83" s="1"/>
+      <c r="R83" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -3734,7 +3729,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
@@ -3742,10 +3737,10 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3760,7 +3755,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
@@ -3768,16 +3763,16 @@
         <v>17</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E86" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -3786,10 +3781,10 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>36</v>
+        <v>256</v>
       </c>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
@@ -3802,25 +3797,23 @@
         <v>15</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-      <c r="H87" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>227</v>
-      </c>
+      <c r="H87" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="I87" s="10"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
@@ -3829,17 +3822,19 @@
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
+      <c r="R87" s="1" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -3860,16 +3855,16 @@
         <v>5</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -3881,12 +3876,8 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q89" s="2" t="s">
-        <v>230</v>
-      </c>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
@@ -3894,10 +3885,10 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
@@ -3909,12 +3900,8 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q90" s="2" t="s">
-        <v>232</v>
-      </c>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
@@ -3922,10 +3909,10 @@
         <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -3938,12 +3925,10 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="5" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="O91" s="1"/>
-      <c r="P91" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
@@ -3952,10 +3937,10 @@
         <v>2</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -3968,12 +3953,10 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O92" s="1"/>
-      <c r="P92" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
@@ -3982,16 +3965,16 @@
         <v>3</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -4002,12 +3985,10 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O93" s="1"/>
-      <c r="P93" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
@@ -4015,8 +3996,12 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
+      <c r="D94" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -4025,11 +4010,11 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
-      <c r="O94" s="1"/>
-      <c r="P94" s="2" t="s">
-        <v>237</v>
-      </c>
+      <c r="N94" s="11"/>
+      <c r="O94" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
@@ -4037,8 +4022,12 @@
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -4047,20 +4036,30 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
-      <c r="O95" s="1"/>
-      <c r="P95" s="2" t="s">
-        <v>238</v>
-      </c>
+      <c r="N95" s="11"/>
+      <c r="O95" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
+      <c r="A96" s="1">
+        <v>4</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -4069,20 +4068,26 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
-      <c r="O96" s="1"/>
-      <c r="P96" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q96" s="1"/>
+      <c r="N96" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O96" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
       <c r="R96" s="1"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
+      <c r="D97" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -4091,11 +4096,11 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
-      <c r="O97" s="1"/>
-      <c r="P97" s="2" t="s">
-        <v>240</v>
-      </c>
+      <c r="N97" s="11"/>
+      <c r="O97" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="P97" s="1"/>
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
@@ -4103,8 +4108,12 @@
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
+      <c r="D98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -4113,18 +4122,24 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="P98" s="2" t="s">
-        <v>241</v>
-      </c>
+      <c r="N98" s="11"/>
+      <c r="O98" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="A99" s="1">
+        <v>6</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4135,72 +4150,89 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1"/>
-      <c r="P99" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q99" s="1"/>
+      <c r="N99" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
       <c r="R99" s="1"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="A100" s="1">
+        <v>1</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
+      <c r="I100" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
-      <c r="P100" s="2" t="s">
-        <v>243</v>
-      </c>
+      <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="A101" s="1">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
+      <c r="I101" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
-      <c r="P101" s="2" t="s">
-        <v>244</v>
-      </c>
+      <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="A102" s="1">
+        <v>3</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
+      <c r="I102" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
@@ -4212,19 +4244,23 @@
       <c r="R102" s="1"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>246</v>
-      </c>
+      <c r="A103" s="1">
+        <v>4</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
+      <c r="I103" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
@@ -4237,50 +4273,48 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
+      <c r="H104" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
-      <c r="N104" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O104" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="P104" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
+      <c r="R104" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="A105" s="1">
+        <v>6</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -4293,18 +4327,22 @@
       <c r="O105" s="1"/>
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
+      <c r="R105" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>250</v>
-      </c>
+      <c r="A106" s="1">
+        <v>7</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
@@ -4317,50 +4355,46 @@
       <c r="O106" s="1"/>
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
-      <c r="R106" s="1"/>
+      <c r="R106" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
-        <v>6</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
+      <c r="H107" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>225</v>
+      </c>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
-      <c r="N107" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="O107" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
+      <c r="R107" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
-        <v>1</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
@@ -4373,20 +4407,20 @@
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
-      <c r="R108" s="1"/>
+      <c r="R108" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>2</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
@@ -4399,20 +4433,20 @@
       <c r="O109" s="1"/>
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
-      <c r="R109" s="1"/>
+      <c r="R109" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
-        <v>3</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
@@ -4425,20 +4459,20 @@
       <c r="O110" s="1"/>
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
+      <c r="R110" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
-        <v>4</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -4451,28 +4485,24 @@
       <c r="O111" s="1"/>
       <c r="P111" s="1"/>
       <c r="Q111" s="1"/>
-      <c r="R111" s="1"/>
+      <c r="R111" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
-        <v>5</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>227</v>
+      </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
-      <c r="H112" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
@@ -4482,18 +4512,18 @@
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
       <c r="R112" s="1" t="s">
-        <v>254</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>255</v>
+        <v>43</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -4510,18 +4540,18 @@
       <c r="P113" s="1"/>
       <c r="Q113" s="1"/>
       <c r="R113" s="1" t="s">
-        <v>38</v>
+        <v>228</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -4538,23 +4568,25 @@
       <c r="P114" s="1"/>
       <c r="Q114" s="1"/>
       <c r="R114" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
+      <c r="A115" s="1">
+        <v>3</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
-      <c r="H115" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="I115" s="7" t="s">
-        <v>258</v>
-      </c>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
@@ -4564,19 +4596,15 @@
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
       <c r="R115" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
-      <c r="D116" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -4585,24 +4613,22 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
-      <c r="N116" s="1"/>
-      <c r="O116" s="1"/>
-      <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
-      <c r="R116" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="N116" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="O116" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
+      <c r="R116" s="1"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
-      <c r="D117" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -4611,221 +4637,13 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
-      <c r="N117" s="1"/>
+      <c r="N117" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="O117" s="1"/>
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
-      <c r="R117" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
-      <c r="J118" s="1"/>
-      <c r="K118" s="1"/>
-      <c r="L118" s="1"/>
-      <c r="M118" s="1"/>
-      <c r="N118" s="1"/>
-      <c r="O118" s="1"/>
-      <c r="P118" s="1"/>
-      <c r="Q118" s="1"/>
-      <c r="R118" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="1"/>
-      <c r="J119" s="1"/>
-      <c r="K119" s="1"/>
-      <c r="L119" s="1"/>
-      <c r="M119" s="1"/>
-      <c r="N119" s="1"/>
-      <c r="O119" s="1"/>
-      <c r="P119" s="1"/>
-      <c r="Q119" s="1"/>
-      <c r="R119" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
-      <c r="J120" s="1"/>
-      <c r="K120" s="1"/>
-      <c r="L120" s="1"/>
-      <c r="M120" s="1"/>
-      <c r="N120" s="1"/>
-      <c r="O120" s="1"/>
-      <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
-      <c r="R120" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A121" s="1">
-        <v>1</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-      <c r="I121" s="1"/>
-      <c r="J121" s="1"/>
-      <c r="K121" s="1"/>
-      <c r="L121" s="1"/>
-      <c r="M121" s="1"/>
-      <c r="N121" s="1"/>
-      <c r="O121" s="1"/>
-      <c r="P121" s="1"/>
-      <c r="Q121" s="1"/>
-      <c r="R121" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A122" s="1">
-        <v>2</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
-      <c r="J122" s="1"/>
-      <c r="K122" s="1"/>
-      <c r="L122" s="1"/>
-      <c r="M122" s="1"/>
-      <c r="N122" s="1"/>
-      <c r="O122" s="1"/>
-      <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
-      <c r="R122" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A123" s="1">
-        <v>3</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-      <c r="I123" s="1"/>
-      <c r="J123" s="1"/>
-      <c r="K123" s="1"/>
-      <c r="L123" s="1"/>
-      <c r="M123" s="1"/>
-      <c r="N123" s="1"/>
-      <c r="O123" s="1"/>
-      <c r="P123" s="1"/>
-      <c r="Q123" s="1"/>
-      <c r="R123" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-      <c r="I124" s="1"/>
-      <c r="J124" s="1"/>
-      <c r="K124" s="1"/>
-      <c r="L124" s="1"/>
-      <c r="M124" s="1"/>
-      <c r="N124" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="O124" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="P124" s="1"/>
-      <c r="Q124" s="1"/>
-      <c r="R124" s="1"/>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
-      <c r="J125" s="1"/>
-      <c r="K125" s="1"/>
-      <c r="L125" s="1"/>
-      <c r="M125" s="1"/>
-      <c r="N125" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="O125" s="1"/>
-      <c r="P125" s="1"/>
-      <c r="Q125" s="1"/>
-      <c r="R125" s="1"/>
+      <c r="R117" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>